<commit_message>
change excel file template for import
</commit_message>
<xml_diff>
--- a/templates/register_form.xlsx
+++ b/templates/register_form.xlsx
@@ -1,144 +1,326 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr codeName="ThisWorkbook"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="465" windowWidth="15015" windowHeight="8100"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Dang ky tim viec" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Migiwa</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Migiwa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pls show "Family Name + First Name"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Migiwa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Pls show "MM/DD/YYYY"</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Migiwa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+When user tick "Viet Nam", import "School Name" here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Migiwa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+When user tick "Nuoc ngoai", import "School Name" here.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AC2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Migiwa:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+When user tick "I'm a fresh graduate", pls show the value of "Just Graduated/No work experience yet" in this field.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
-  <si>
-    <t>Tên</t>
-  </si>
-  <si>
-    <t>Phiên âm tên</t>
-  </si>
-  <si>
-    <t>Tuổi</t>
-  </si>
-  <si>
-    <t>Giới tính</t>
-  </si>
-  <si>
-    <t>Ngày tháng năm sinh</t>
-  </si>
-  <si>
-    <t>Địa chỉ</t>
-  </si>
-  <si>
-    <t>Điện thoại</t>
-  </si>
-  <si>
-    <t>Đã kết hôn/Độc thân</t>
-  </si>
-  <si>
-    <t>Điên thoại di động</t>
-  </si>
-  <si>
-    <t>Quốc tịch</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>Tên trường đại học/Khoa</t>
-  </si>
-  <si>
-    <t>Năm nhập học～Năm tốt nghiệp</t>
-  </si>
-  <si>
-    <t>Bằng cấp Nhật ngữ</t>
-  </si>
-  <si>
-    <t>Khả năng hội thoại</t>
-  </si>
-  <si>
-    <t>Khả năng đọc hiểu</t>
-  </si>
-  <si>
-    <t>Bằng cấp tiếng Anh</t>
-  </si>
-  <si>
-    <t>Bằng cấp tiếng Việt</t>
-  </si>
-  <si>
-    <t>WORD</t>
-  </si>
-  <si>
-    <t>EXCEL</t>
-  </si>
-  <si>
-    <t>Năng lực/bằng cấp khác</t>
-  </si>
-  <si>
-    <t>Công việc/tình trạng chuyển chỗ làm</t>
-  </si>
-  <si>
-    <t>Tình trạng công việc hiện tại</t>
-  </si>
-  <si>
-    <t>Thu nhập hiện tai</t>
-  </si>
-  <si>
-    <t>Nguyện vọng trợ cấp</t>
-  </si>
-  <si>
-    <t>Kinh nghiệm nghiệp vụ</t>
-  </si>
-  <si>
-    <t>Loại công việc ứng dụng</t>
-  </si>
-  <si>
-    <t>Nguyện vọng bản thân</t>
-  </si>
-  <si>
-    <t>Cơ hội nào biết công ty chúng tôi</t>
-  </si>
-  <si>
-    <t>Ngày đăng ký</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>E-mail</t>
+  </si>
+  <si>
+    <t>Current Salary</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Expected Salary</t>
+  </si>
+  <si>
+    <t>Expected Industry</t>
+  </si>
+  <si>
+    <t>Expected Function</t>
+  </si>
+  <si>
+    <t>Expected Location</t>
+  </si>
+  <si>
+    <t>Expected job level</t>
+  </si>
+  <si>
+    <t>VN  School</t>
+  </si>
+  <si>
+    <t>Oversea School</t>
+  </si>
+  <si>
+    <t>Faculty</t>
+  </si>
+  <si>
+    <t>Degree</t>
+  </si>
+  <si>
+    <t>Graduation Year</t>
+  </si>
+  <si>
+    <t>Experienced Industry</t>
+  </si>
+  <si>
+    <t>Experienced Function</t>
+  </si>
+  <si>
+    <t>Experienced Job Level</t>
+  </si>
+  <si>
+    <t>Experience Year</t>
+  </si>
+  <si>
+    <t>Experience Details</t>
+  </si>
+  <si>
+    <t>Japanese level</t>
+  </si>
+  <si>
+    <t>English level</t>
+  </si>
+  <si>
+    <t>Vietnamese level</t>
+  </si>
+  <si>
+    <t>Other language proficiency</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>When change job?</t>
+  </si>
+  <si>
+    <t>General Information</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Birthday</t>
+  </si>
+  <si>
+    <t>Expectations</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Working Experience</t>
+  </si>
+  <si>
+    <t>Language and Skill</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Registration Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="6"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -146,19 +328,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -208,10 +475,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="?? ?????"/>
-        <a:font script="Hang" typeface="?? ??"/>
-        <a:font script="Hans" typeface="??"/>
-        <a:font script="Hant" typeface="????"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -237,15 +504,16 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="?? ?????"/>
-        <a:font script="Hang" typeface="?? ??"/>
-        <a:font script="Hans" typeface="??"/>
-        <a:font script="Hant" typeface="????"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -271,6 +539,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -446,156 +715,251 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AJ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="29" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="24" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.85546875" customWidth="1"/>
+    <col min="29" max="29" width="24" customWidth="1"/>
+    <col min="36" max="36" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="8"/>
+      <c r="AD1" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="AE1" s="10"/>
+      <c r="AF1" s="10"/>
+      <c r="AG1" s="10"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ1" s="3"/>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W1" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AE2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH2" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AI2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+      <c r="AB3" s="1"/>
+      <c r="AC3" s="1"/>
+      <c r="AD3" s="1"/>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1"/>
+      <c r="AG3" s="1"/>
+      <c r="AH3" s="1"/>
+      <c r="AI3" s="1"/>
+      <c r="AJ3" s="1"/>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <phoneticPr fontId="2"/>
+  <mergeCells count="5">
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="Y1:AC1"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="M1:S1"/>
+    <mergeCell ref="T1:X1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>